<commit_message>
Adicionando pre-escrita do relatorio.
</commit_message>
<xml_diff>
--- a/Trabalho Etapa II (EXPERIMENTAL)/Ensaios_Sistema/medicoes.xlsx
+++ b/Trabalho Etapa II (EXPERIMENTAL)/Ensaios_Sistema/medicoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebrain\Desktop\Controle-Digital-Etapa-Experimental\Trabalho Etapa II (EXPERIMENTAL)\Ensaios_Sistema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B628EB74-3A09-4BE4-A63D-A72E05920268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038991AE-661F-4AC2-B51C-323EB2E15BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1039,9 +1039,9 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1372,7 +1372,7 @@
   <dimension ref="A1:N1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>